<commit_message>
Update with Agile Methodology
</commit_message>
<xml_diff>
--- a/VocationEvaluationMatrix_v1.xlsx
+++ b/VocationEvaluationMatrix_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petrusk\Desktop\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8C3E01-1729-4B2B-8F1E-1B7F16489601}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC878C5-F7AA-4651-B018-443B73B57071}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68A18233-E500-41A9-8445-D8FE700CC7BE}"/>
+    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15840" xr2:uid="{68A18233-E500-41A9-8445-D8FE700CC7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Points</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>next vocation/company</t>
+  </si>
+  <si>
+    <t>Agile/Scrum Methodology</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
   <dimension ref="B1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,19 +1042,21 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" s="15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D18" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F18" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H18" s="13"/>
     </row>
@@ -1097,7 +1102,7 @@
       <c r="B21" s="16"/>
       <c r="C21" s="17">
         <f>SUM(C3:C20)</f>
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D21" s="17">
         <f>SUM(D3:D20)</f>
@@ -1110,7 +1115,7 @@
       </c>
       <c r="G21" s="17">
         <f>SUM(G3:G20)</f>
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="H21" s="19"/>
     </row>

</xml_diff>